<commit_message>
corrections to excel files
</commit_message>
<xml_diff>
--- a/Testdata/Objectrepo/objectrepo.xlsx
+++ b/Testdata/Objectrepo/objectrepo.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="38">
   <si>
     <t>pagename</t>
   </si>
@@ -69,6 +69,66 @@
   </si>
   <si>
     <t>//a[@id="topTabFT"]</t>
+  </si>
+  <si>
+    <t>maintain_batch_template</t>
+  </si>
+  <si>
+    <t>//a[text()="Maintain Batch Template"]</t>
+  </si>
+  <si>
+    <t>add_new</t>
+  </si>
+  <si>
+    <t>//a[@id="addNewButton"]</t>
+  </si>
+  <si>
+    <t>template_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> //input[@name='tname']</t>
+  </si>
+  <si>
+    <t>template_desc</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> //input[@name='tdesc']</t>
+  </si>
+  <si>
+    <t>ACH_batch_class</t>
+  </si>
+  <si>
+    <t>//select[@name='batchClass']</t>
+  </si>
+  <si>
+    <t>ACH_batch_class_option</t>
+  </si>
+  <si>
+    <t>//select[@name='batchClass']/option[@value="PPD"]</t>
+  </si>
+  <si>
+    <t>ACH_ID</t>
+  </si>
+  <si>
+    <t>//select[@name='achid']</t>
+  </si>
+  <si>
+    <t>ACH_ID_option</t>
+  </si>
+  <si>
+    <t>//select[@name='achid']/option[@value="TESTID"]</t>
+  </si>
+  <si>
+    <t>Create_offsetting_transaction</t>
+  </si>
+  <si>
+    <t>//input[@name='offsetTrans']</t>
+  </si>
+  <si>
+    <t>add_button</t>
+  </si>
+  <si>
+    <t>//a[@id='addButton']</t>
   </si>
 </sst>
 </file>
@@ -77,9 +137,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -100,20 +160,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
@@ -121,6 +167,36 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -128,8 +204,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -143,47 +236,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -213,46 +281,38 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -273,13 +333,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -291,67 +483,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -363,97 +507,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -483,25 +543,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -521,6 +572,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -536,17 +596,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -556,6 +610,21 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -570,150 +639,141 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1119,10 +1179,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="$A7:$XFD16"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -1244,17 +1304,200 @@
       </c>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="2:3">
-      <c r="B7" s="5"/>
-      <c r="C7" s="3"/>
-    </row>
-    <row r="8" spans="2:3">
-      <c r="B8" s="5"/>
-      <c r="C8" s="3"/>
-    </row>
-    <row r="9" spans="2:3">
-      <c r="B9" s="5"/>
-      <c r="C9" s="3"/>
+    <row r="7" customFormat="1" spans="1:6">
+      <c r="A7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" customFormat="1" spans="1:6">
+      <c r="A8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" customFormat="1" spans="1:6">
+      <c r="A9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" customFormat="1" spans="1:6">
+      <c r="A10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" customFormat="1" spans="1:6">
+      <c r="A11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" customFormat="1" spans="1:6">
+      <c r="A12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" customFormat="1" spans="1:6">
+      <c r="A13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" customFormat="1" spans="1:6">
+      <c r="A14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
first draft for new batch template workflow
</commit_message>
<xml_diff>
--- a/Testdata/Objectrepo/objectrepo.xlsx
+++ b/Testdata/Objectrepo/objectrepo.xlsx
@@ -86,13 +86,13 @@
     <t>template_name</t>
   </si>
   <si>
-    <t xml:space="preserve"> //input[@name='tname']</t>
+    <t>//input[@name='tname']</t>
   </si>
   <si>
     <t>template_desc</t>
   </si>
   <si>
-    <t xml:space="preserve"> //input[@name='tdesc']</t>
+    <t>//input[@name='tdesc']</t>
   </si>
   <si>
     <t>ACH_batch_class</t>
@@ -136,10 +136,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -160,6 +160,14 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
@@ -167,54 +175,38 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -244,13 +236,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -281,6 +266,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -288,31 +281,38 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -333,25 +333,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -363,13 +495,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -381,139 +507,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -599,15 +599,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
@@ -639,141 +630,150 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1182,7 +1182,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54285714285714" defaultRowHeight="15" outlineLevelCol="5"/>

</xml_diff>